<commit_message>
Add fiew Tables to databese
</commit_message>
<xml_diff>
--- a/GPERP_APP/Resources/Templates/Karta_pracy.xlsx
+++ b/GPERP_APP/Resources/Templates/Karta_pracy.xlsx
@@ -5,16 +5,19 @@
   <workbookPr codeName="Ten_skoroszyt" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\projekty GitHub\GlassPlant-ERP\GPERP_APP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\projekty GitHub\GlassPlant-ERP\GPERP_APP\Resources\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999615D0-BC01-4FFA-B134-B89B0D126DD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6A31E4-4163-445A-901C-B85024D10C0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="19212" windowHeight="9792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Karta" sheetId="4" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Karta!$A$1:$AL$24</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -574,47 +577,47 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
@@ -646,38 +649,38 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1224,7 +1227,7 @@
   <dimension ref="A1:IV24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1240,46 +1243,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="27" customHeight="1">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="65"/>
-      <c r="AB1" s="65"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="66"/>
-      <c r="AG1" s="66"/>
-      <c r="AH1" s="66"/>
-      <c r="AI1" s="66"/>
-      <c r="AJ1" s="66"/>
-      <c r="AK1" s="66"/>
-      <c r="AL1" s="66"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
+      <c r="AL1" s="36"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
@@ -1500,52 +1503,52 @@
       <c r="IV1" s="1"/>
     </row>
     <row r="2" spans="1:256" ht="9.75" customHeight="1">
-      <c r="A2" s="63"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="67" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67" t="s">
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="67"/>
-      <c r="T2" s="67"/>
-      <c r="U2" s="67"/>
-      <c r="V2" s="67"/>
-      <c r="W2" s="67"/>
-      <c r="X2" s="67"/>
-      <c r="Y2" s="67"/>
-      <c r="Z2" s="67"/>
-      <c r="AA2" s="67"/>
-      <c r="AB2" s="67"/>
-      <c r="AC2" s="67" t="s">
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="AD2" s="67"/>
-      <c r="AE2" s="67"/>
-      <c r="AF2" s="67"/>
-      <c r="AG2" s="67"/>
-      <c r="AH2" s="67"/>
-      <c r="AI2" s="67" t="s">
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="37"/>
+      <c r="AI2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="AJ2" s="67"/>
-      <c r="AK2" s="67"/>
-      <c r="AL2" s="67"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="37"/>
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
@@ -1766,48 +1769,48 @@
       <c r="IV2" s="1"/>
     </row>
     <row r="3" spans="1:256" ht="18" customHeight="1">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59" t="s">
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="59"/>
-      <c r="R3" s="59"/>
-      <c r="S3" s="59"/>
-      <c r="T3" s="59"/>
-      <c r="U3" s="59"/>
-      <c r="V3" s="59"/>
-      <c r="W3" s="59"/>
-      <c r="X3" s="59"/>
-      <c r="Y3" s="59"/>
-      <c r="Z3" s="59"/>
-      <c r="AA3" s="59"/>
-      <c r="AB3" s="59"/>
-      <c r="AC3" s="59"/>
-      <c r="AD3" s="59"/>
-      <c r="AE3" s="59"/>
-      <c r="AF3" s="59"/>
-      <c r="AG3" s="59"/>
-      <c r="AH3" s="59"/>
-      <c r="AI3" s="59"/>
-      <c r="AJ3" s="59"/>
-      <c r="AK3" s="59"/>
-      <c r="AL3" s="59"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
+      <c r="V3" s="38"/>
+      <c r="W3" s="38"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="38"/>
+      <c r="AB3" s="38"/>
+      <c r="AC3" s="38"/>
+      <c r="AD3" s="38"/>
+      <c r="AE3" s="38"/>
+      <c r="AF3" s="38"/>
+      <c r="AG3" s="38"/>
+      <c r="AH3" s="38"/>
+      <c r="AI3" s="38"/>
+      <c r="AJ3" s="38"/>
+      <c r="AK3" s="38"/>
+      <c r="AL3" s="38"/>
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
@@ -2028,52 +2031,52 @@
       <c r="IV3" s="1"/>
     </row>
     <row r="4" spans="1:256" ht="14.85" customHeight="1">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="61" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="61"/>
-      <c r="P4" s="61"/>
-      <c r="Q4" s="61"/>
-      <c r="R4" s="61"/>
-      <c r="S4" s="61"/>
-      <c r="T4" s="61"/>
-      <c r="U4" s="61"/>
-      <c r="V4" s="61"/>
-      <c r="W4" s="61"/>
-      <c r="X4" s="61"/>
-      <c r="Y4" s="61"/>
-      <c r="Z4" s="61"/>
-      <c r="AA4" s="61"/>
-      <c r="AB4" s="61"/>
-      <c r="AC4" s="61"/>
-      <c r="AD4" s="61"/>
-      <c r="AE4" s="61"/>
-      <c r="AF4" s="61"/>
-      <c r="AG4" s="61"/>
-      <c r="AH4" s="61"/>
-      <c r="AI4" s="61" t="s">
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="40"/>
+      <c r="X4" s="40"/>
+      <c r="Y4" s="40"/>
+      <c r="Z4" s="40"/>
+      <c r="AA4" s="40"/>
+      <c r="AB4" s="40"/>
+      <c r="AC4" s="40"/>
+      <c r="AD4" s="40"/>
+      <c r="AE4" s="40"/>
+      <c r="AF4" s="40"/>
+      <c r="AG4" s="40"/>
+      <c r="AH4" s="40"/>
+      <c r="AI4" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="AJ4" s="62" t="s">
+      <c r="AJ4" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="AK4" s="62"/>
-      <c r="AL4" s="62" t="s">
+      <c r="AK4" s="41"/>
+      <c r="AL4" s="41" t="s">
         <v>10</v>
       </c>
       <c r="AM4" s="2"/>
@@ -2296,9 +2299,9 @@
       <c r="IV4" s="2"/>
     </row>
     <row r="5" spans="1:256" s="4" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A5" s="60"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
       <c r="D5" s="32"/>
       <c r="E5" s="32"/>
       <c r="F5" s="32"/>
@@ -2330,10 +2333,10 @@
       <c r="AF5" s="32"/>
       <c r="AG5" s="32"/>
       <c r="AH5" s="32"/>
-      <c r="AI5" s="61"/>
-      <c r="AJ5" s="62"/>
-      <c r="AK5" s="62"/>
-      <c r="AL5" s="62"/>
+      <c r="AI5" s="40"/>
+      <c r="AJ5" s="41"/>
+      <c r="AK5" s="41"/>
+      <c r="AL5" s="41"/>
       <c r="AM5" s="3"/>
       <c r="AN5" s="3"/>
       <c r="AO5" s="3"/>
@@ -2554,11 +2557,11 @@
       <c r="IV5" s="3"/>
     </row>
     <row r="6" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="57"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="29"/>
       <c r="E6" s="29"/>
       <c r="F6" s="29"/>
@@ -2591,10 +2594,10 @@
       <c r="AG6" s="29"/>
       <c r="AH6" s="29"/>
       <c r="AI6" s="11"/>
-      <c r="AJ6" s="38" t="s">
+      <c r="AJ6" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="AK6" s="38"/>
+      <c r="AK6" s="44"/>
       <c r="AL6" s="5"/>
       <c r="AM6" s="1"/>
       <c r="AN6" s="1"/>
@@ -2816,11 +2819,11 @@
       <c r="IV6" s="1"/>
     </row>
     <row r="7" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="30"/>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
@@ -2853,8 +2856,8 @@
       <c r="AG7" s="30"/>
       <c r="AH7" s="30"/>
       <c r="AI7" s="11"/>
-      <c r="AJ7" s="34"/>
-      <c r="AK7" s="34"/>
+      <c r="AJ7" s="45"/>
+      <c r="AK7" s="45"/>
       <c r="AL7" s="6"/>
       <c r="AM7" s="1"/>
       <c r="AN7" s="1"/>
@@ -3076,9 +3079,9 @@
       <c r="IV7" s="1"/>
     </row>
     <row r="8" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A8" s="58"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="58"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="31"/>
       <c r="E8" s="31"/>
       <c r="F8" s="31"/>
@@ -3111,10 +3114,10 @@
       <c r="AG8" s="31"/>
       <c r="AH8" s="31"/>
       <c r="AI8" s="11"/>
-      <c r="AJ8" s="38" t="s">
+      <c r="AJ8" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="AK8" s="38"/>
+      <c r="AK8" s="44"/>
       <c r="AL8" s="6"/>
       <c r="AM8" s="1"/>
       <c r="AN8" s="1"/>
@@ -3371,8 +3374,8 @@
       <c r="AG9" s="20"/>
       <c r="AH9" s="20"/>
       <c r="AI9" s="10"/>
-      <c r="AJ9" s="34"/>
-      <c r="AK9" s="34"/>
+      <c r="AJ9" s="45"/>
+      <c r="AK9" s="45"/>
       <c r="AL9" s="7"/>
       <c r="AM9" s="1"/>
       <c r="AN9" s="1"/>
@@ -3629,8 +3632,8 @@
       <c r="AG10" s="24"/>
       <c r="AH10" s="24"/>
       <c r="AI10" s="10"/>
-      <c r="AJ10" s="34"/>
-      <c r="AK10" s="34"/>
+      <c r="AJ10" s="45"/>
+      <c r="AK10" s="45"/>
       <c r="AL10" s="5"/>
       <c r="AM10" s="1"/>
       <c r="AN10" s="1"/>
@@ -4112,11 +4115,11 @@
       <c r="IV11" s="1"/>
     </row>
     <row r="12" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
       <c r="D12" s="25"/>
       <c r="E12" s="26"/>
       <c r="F12" s="26"/>
@@ -4149,10 +4152,10 @@
       <c r="AG12" s="26"/>
       <c r="AH12" s="26"/>
       <c r="AI12" s="15"/>
-      <c r="AJ12" s="41" t="s">
+      <c r="AJ12" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="AK12" s="42"/>
+      <c r="AK12" s="59"/>
       <c r="AL12" s="18"/>
       <c r="AM12" s="1"/>
       <c r="AN12" s="1"/>
@@ -4374,13 +4377,13 @@
       <c r="IV12" s="1"/>
     </row>
     <row r="13" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="45"/>
+      <c r="C13" s="62"/>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
@@ -4413,10 +4416,10 @@
       <c r="AG13" s="27"/>
       <c r="AH13" s="27"/>
       <c r="AI13" s="14"/>
-      <c r="AJ13" s="46" t="s">
+      <c r="AJ13" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="AK13" s="46"/>
+      <c r="AK13" s="63"/>
       <c r="AL13" s="17"/>
       <c r="AM13" s="1"/>
       <c r="AN13" s="1"/>
@@ -4638,11 +4641,11 @@
       <c r="IV13" s="1"/>
     </row>
     <row r="14" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A14" s="44"/>
-      <c r="B14" s="38" t="s">
+      <c r="A14" s="61"/>
+      <c r="B14" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="38"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -4675,10 +4678,10 @@
       <c r="AG14" s="10"/>
       <c r="AH14" s="10"/>
       <c r="AI14" s="10"/>
-      <c r="AJ14" s="38" t="s">
+      <c r="AJ14" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="AK14" s="38"/>
+      <c r="AK14" s="44"/>
       <c r="AL14" s="8"/>
       <c r="AM14" s="1"/>
       <c r="AN14" s="1"/>
@@ -4900,11 +4903,11 @@
       <c r="IV14" s="1"/>
     </row>
     <row r="15" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A15" s="44"/>
-      <c r="B15" s="38" t="s">
+      <c r="A15" s="61"/>
+      <c r="B15" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="38"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -4937,10 +4940,10 @@
       <c r="AG15" s="10"/>
       <c r="AH15" s="10"/>
       <c r="AI15" s="10"/>
-      <c r="AJ15" s="38" t="s">
+      <c r="AJ15" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="AK15" s="38"/>
+      <c r="AK15" s="44"/>
       <c r="AL15" s="5"/>
       <c r="AM15" s="1"/>
       <c r="AN15" s="1"/>
@@ -5162,11 +5165,11 @@
       <c r="IV15" s="1"/>
     </row>
     <row r="16" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A16" s="44"/>
-      <c r="B16" s="38" t="s">
+      <c r="A16" s="61"/>
+      <c r="B16" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="38"/>
+      <c r="C16" s="44"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -5199,10 +5202,10 @@
       <c r="AG16" s="10"/>
       <c r="AH16" s="10"/>
       <c r="AI16" s="10"/>
-      <c r="AJ16" s="38" t="s">
+      <c r="AJ16" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="AK16" s="38"/>
+      <c r="AK16" s="44"/>
       <c r="AL16" s="5"/>
       <c r="AM16" s="1"/>
       <c r="AN16" s="1"/>
@@ -5424,11 +5427,11 @@
       <c r="IV16" s="1"/>
     </row>
     <row r="17" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A17" s="44"/>
-      <c r="B17" s="38" t="s">
+      <c r="A17" s="61"/>
+      <c r="B17" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="38"/>
+      <c r="C17" s="44"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -5461,10 +5464,10 @@
       <c r="AG17" s="10"/>
       <c r="AH17" s="10"/>
       <c r="AI17" s="10"/>
-      <c r="AJ17" s="38" t="s">
+      <c r="AJ17" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="AK17" s="38"/>
+      <c r="AK17" s="44"/>
       <c r="AL17" s="5"/>
       <c r="AM17" s="1"/>
       <c r="AN17" s="1"/>
@@ -5686,11 +5689,11 @@
       <c r="IV17" s="1"/>
     </row>
     <row r="18" spans="1:256" ht="24.75" customHeight="1">
-      <c r="A18" s="44"/>
-      <c r="B18" s="33" t="s">
+      <c r="A18" s="61"/>
+      <c r="B18" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="33"/>
+      <c r="C18" s="42"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -5723,10 +5726,10 @@
       <c r="AG18" s="10"/>
       <c r="AH18" s="10"/>
       <c r="AI18" s="10"/>
-      <c r="AJ18" s="33" t="s">
+      <c r="AJ18" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="AK18" s="33"/>
+      <c r="AK18" s="42"/>
       <c r="AL18" s="5"/>
       <c r="AM18" s="1"/>
       <c r="AN18" s="1"/>
@@ -5948,11 +5951,11 @@
       <c r="IV18" s="1"/>
     </row>
     <row r="19" spans="1:256" ht="24.75" customHeight="1">
-      <c r="A19" s="44"/>
-      <c r="B19" s="33" t="s">
+      <c r="A19" s="61"/>
+      <c r="B19" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="33"/>
+      <c r="C19" s="42"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -5985,10 +5988,10 @@
       <c r="AG19" s="10"/>
       <c r="AH19" s="10"/>
       <c r="AI19" s="10"/>
-      <c r="AJ19" s="33" t="s">
+      <c r="AJ19" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="AK19" s="33"/>
+      <c r="AK19" s="42"/>
       <c r="AL19" s="5"/>
       <c r="AM19" s="1"/>
       <c r="AN19" s="1"/>
@@ -6210,11 +6213,11 @@
       <c r="IV19" s="1"/>
     </row>
     <row r="20" spans="1:256" ht="24.75" customHeight="1">
-      <c r="A20" s="44"/>
-      <c r="B20" s="37" t="s">
+      <c r="A20" s="61"/>
+      <c r="B20" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="37"/>
+      <c r="C20" s="66"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -6247,8 +6250,8 @@
       <c r="AG20" s="10"/>
       <c r="AH20" s="10"/>
       <c r="AI20" s="10"/>
-      <c r="AJ20" s="34"/>
-      <c r="AK20" s="34"/>
+      <c r="AJ20" s="45"/>
+      <c r="AK20" s="45"/>
       <c r="AL20" s="5"/>
       <c r="AM20" s="1"/>
       <c r="AN20" s="1"/>
@@ -6470,45 +6473,45 @@
       <c r="IV20" s="1"/>
     </row>
     <row r="21" spans="1:256" ht="17.25" customHeight="1">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="39"/>
-      <c r="R21" s="39"/>
-      <c r="S21" s="39"/>
-      <c r="T21" s="39"/>
-      <c r="U21" s="39"/>
-      <c r="V21" s="39"/>
-      <c r="W21" s="39"/>
-      <c r="X21" s="39"/>
-      <c r="Y21" s="39"/>
-      <c r="Z21" s="39"/>
-      <c r="AA21" s="39"/>
-      <c r="AB21" s="39"/>
-      <c r="AC21" s="39"/>
-      <c r="AD21" s="39"/>
-      <c r="AE21" s="39"/>
-      <c r="AF21" s="39"/>
-      <c r="AG21" s="39"/>
-      <c r="AH21" s="39"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="67"/>
+      <c r="M21" s="67"/>
+      <c r="N21" s="67"/>
+      <c r="O21" s="67"/>
+      <c r="P21" s="67"/>
+      <c r="Q21" s="67"/>
+      <c r="R21" s="67"/>
+      <c r="S21" s="67"/>
+      <c r="T21" s="67"/>
+      <c r="U21" s="67"/>
+      <c r="V21" s="67"/>
+      <c r="W21" s="67"/>
+      <c r="X21" s="67"/>
+      <c r="Y21" s="67"/>
+      <c r="Z21" s="67"/>
+      <c r="AA21" s="67"/>
+      <c r="AB21" s="67"/>
+      <c r="AC21" s="67"/>
+      <c r="AD21" s="67"/>
+      <c r="AE21" s="67"/>
+      <c r="AF21" s="67"/>
+      <c r="AG21" s="67"/>
+      <c r="AH21" s="67"/>
       <c r="AI21" s="13"/>
-      <c r="AJ21" s="34"/>
-      <c r="AK21" s="34"/>
+      <c r="AJ21" s="45"/>
+      <c r="AK21" s="45"/>
       <c r="AL21" s="5"/>
       <c r="AM21" s="1"/>
       <c r="AN21" s="1"/>
@@ -6730,43 +6733,43 @@
       <c r="IV21" s="1"/>
     </row>
     <row r="22" spans="1:256" ht="15.75" customHeight="1">
-      <c r="A22" s="38"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="39"/>
-      <c r="O22" s="39"/>
-      <c r="P22" s="39"/>
-      <c r="Q22" s="39"/>
-      <c r="R22" s="39"/>
-      <c r="S22" s="39"/>
-      <c r="T22" s="39"/>
-      <c r="U22" s="39"/>
-      <c r="V22" s="39"/>
-      <c r="W22" s="39"/>
-      <c r="X22" s="39"/>
-      <c r="Y22" s="39"/>
-      <c r="Z22" s="39"/>
-      <c r="AA22" s="39"/>
-      <c r="AB22" s="39"/>
-      <c r="AC22" s="39"/>
-      <c r="AD22" s="39"/>
-      <c r="AE22" s="39"/>
-      <c r="AF22" s="39"/>
-      <c r="AG22" s="39"/>
-      <c r="AH22" s="39"/>
+      <c r="A22" s="44"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="67"/>
+      <c r="M22" s="67"/>
+      <c r="N22" s="67"/>
+      <c r="O22" s="67"/>
+      <c r="P22" s="67"/>
+      <c r="Q22" s="67"/>
+      <c r="R22" s="67"/>
+      <c r="S22" s="67"/>
+      <c r="T22" s="67"/>
+      <c r="U22" s="67"/>
+      <c r="V22" s="67"/>
+      <c r="W22" s="67"/>
+      <c r="X22" s="67"/>
+      <c r="Y22" s="67"/>
+      <c r="Z22" s="67"/>
+      <c r="AA22" s="67"/>
+      <c r="AB22" s="67"/>
+      <c r="AC22" s="67"/>
+      <c r="AD22" s="67"/>
+      <c r="AE22" s="67"/>
+      <c r="AF22" s="67"/>
+      <c r="AG22" s="67"/>
+      <c r="AH22" s="67"/>
       <c r="AI22" s="10"/>
-      <c r="AJ22" s="34"/>
-      <c r="AK22" s="34"/>
+      <c r="AJ22" s="45"/>
+      <c r="AK22" s="45"/>
       <c r="AL22" s="5"/>
       <c r="AM22" s="1"/>
       <c r="AN22" s="1"/>
@@ -6988,138 +6991,45 @@
       <c r="IV22" s="1"/>
     </row>
     <row r="23" spans="1:256" ht="18.75" customHeight="1">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="10">
-        <f>SUM(D8:D10,D12:D20)</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="10">
-        <f t="shared" ref="E23:AH23" si="0">SUM(E8:E10,E12:E20)</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="X23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Y23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Z23" s="10">
-        <f>SUM(Z8:Z10,Z12:Z20)</f>
-        <v>0</v>
-      </c>
-      <c r="AA23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AB23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AC23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AE23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AF23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AG23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AH23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="10"/>
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="10"/>
+      <c r="AB23" s="10"/>
+      <c r="AC23" s="10"/>
+      <c r="AD23" s="10"/>
+      <c r="AE23" s="10"/>
+      <c r="AF23" s="10"/>
+      <c r="AG23" s="10"/>
+      <c r="AH23" s="10"/>
       <c r="AI23" s="10"/>
-      <c r="AJ23" s="34"/>
-      <c r="AK23" s="34"/>
+      <c r="AJ23" s="45"/>
+      <c r="AK23" s="45"/>
       <c r="AL23" s="5"/>
       <c r="AM23" s="1"/>
       <c r="AN23" s="1"/>
@@ -7341,47 +7251,47 @@
       <c r="IV23" s="1"/>
     </row>
     <row r="24" spans="1:256" ht="23.4" customHeight="1">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="35"/>
-      <c r="P24" s="35"/>
-      <c r="Q24" s="35"/>
-      <c r="R24" s="35"/>
-      <c r="S24" s="35"/>
-      <c r="T24" s="35"/>
-      <c r="U24" s="35"/>
-      <c r="V24" s="35"/>
-      <c r="W24" s="35"/>
-      <c r="X24" s="35"/>
-      <c r="Y24" s="35"/>
-      <c r="Z24" s="35"/>
-      <c r="AA24" s="35"/>
-      <c r="AB24" s="35"/>
-      <c r="AC24" s="35"/>
-      <c r="AD24" s="35"/>
-      <c r="AE24" s="35"/>
-      <c r="AF24" s="35"/>
-      <c r="AG24" s="35"/>
-      <c r="AH24" s="35"/>
-      <c r="AI24" s="35"/>
-      <c r="AJ24" s="36" t="s">
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="64"/>
+      <c r="J24" s="64"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64"/>
+      <c r="O24" s="64"/>
+      <c r="P24" s="64"/>
+      <c r="Q24" s="64"/>
+      <c r="R24" s="64"/>
+      <c r="S24" s="64"/>
+      <c r="T24" s="64"/>
+      <c r="U24" s="64"/>
+      <c r="V24" s="64"/>
+      <c r="W24" s="64"/>
+      <c r="X24" s="64"/>
+      <c r="Y24" s="64"/>
+      <c r="Z24" s="64"/>
+      <c r="AA24" s="64"/>
+      <c r="AB24" s="64"/>
+      <c r="AC24" s="64"/>
+      <c r="AD24" s="64"/>
+      <c r="AE24" s="64"/>
+      <c r="AF24" s="64"/>
+      <c r="AG24" s="64"/>
+      <c r="AH24" s="64"/>
+      <c r="AI24" s="64"/>
+      <c r="AJ24" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="AK24" s="36"/>
+      <c r="AK24" s="65"/>
       <c r="AL24" s="5"/>
       <c r="AM24" s="1"/>
       <c r="AN24" s="1"/>
@@ -7604,35 +7514,17 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="A1:F2"/>
-    <mergeCell ref="G1:L1"/>
-    <mergeCell ref="M1:AB1"/>
-    <mergeCell ref="AC1:AH1"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="M2:AB2"/>
-    <mergeCell ref="AC2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="M3:AL3"/>
-    <mergeCell ref="A4:C5"/>
-    <mergeCell ref="D4:AH4"/>
-    <mergeCell ref="AI4:AI5"/>
-    <mergeCell ref="AJ4:AK5"/>
-    <mergeCell ref="AL4:AL5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="AJ6:AK6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="AJ7:AK7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="AJ8:AK8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="AJ9:AK9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="AJ10:AK10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:AH11"/>
-    <mergeCell ref="AJ11:AK11"/>
+    <mergeCell ref="AJ19:AK19"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="AJ23:AK23"/>
+    <mergeCell ref="A24:AI24"/>
+    <mergeCell ref="AJ24:AK24"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="AJ20:AK20"/>
+    <mergeCell ref="A21:C22"/>
+    <mergeCell ref="D21:AH22"/>
+    <mergeCell ref="AJ21:AK21"/>
+    <mergeCell ref="AJ22:AK22"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="AJ12:AK12"/>
     <mergeCell ref="A13:A20"/>
@@ -7649,17 +7541,35 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="AJ18:AK18"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="AJ19:AK19"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="AJ23:AK23"/>
-    <mergeCell ref="A24:AI24"/>
-    <mergeCell ref="AJ24:AK24"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="AJ20:AK20"/>
-    <mergeCell ref="A21:C22"/>
-    <mergeCell ref="D21:AH22"/>
-    <mergeCell ref="AJ21:AK21"/>
-    <mergeCell ref="AJ22:AK22"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="AJ9:AK9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="AJ10:AK10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:AH11"/>
+    <mergeCell ref="AJ11:AK11"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="AJ6:AK6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="AJ7:AK7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="AJ8:AK8"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="M3:AL3"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="D4:AH4"/>
+    <mergeCell ref="AI4:AI5"/>
+    <mergeCell ref="AJ4:AK5"/>
+    <mergeCell ref="AL4:AL5"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="M1:AB1"/>
+    <mergeCell ref="AC1:AH1"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="M2:AB2"/>
+    <mergeCell ref="AC2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
   </mergeCells>
   <conditionalFormatting sqref="D23:AH23">
     <cfRule type="cellIs" dxfId="36" priority="196" operator="equal">

</xml_diff>

<commit_message>
Some updates in HumanResources
</commit_message>
<xml_diff>
--- a/GPERP_APP/Resources/Templates/Karta_pracy.xlsx
+++ b/GPERP_APP/Resources/Templates/Karta_pracy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr codeName="Ten_skoroszyt" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\projekty GitHub\GlassPlant-ERP\GPERP_APP\Resources\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6A31E4-4163-445A-901C-B85024D10C0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C326F0C-2D2D-4AF0-962D-66C5B1C12EB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="19212" windowHeight="9792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Karta" sheetId="4" r:id="rId1"/>
@@ -122,23 +122,24 @@
     <t>Nieobecność nieusprawiedliwiona</t>
   </si>
   <si>
-    <t>Sporządził: xxxxxxxxx</t>
-  </si>
-  <si>
     <t>rok</t>
   </si>
   <si>
     <t xml:space="preserve">Od godz. </t>
+  </si>
+  <si>
+    <t>Sporządził: Wit Łuczyński</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;[$zł-415];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$zł-415]"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;zł&quot;"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,12 +238,6 @@
       <charset val="238"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial1"/>
-      <charset val="238"/>
-    </font>
-    <font>
       <sz val="7"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -260,6 +255,20 @@
     <font>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Arial1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Arial1"/>
       <charset val="238"/>
     </font>
@@ -481,7 +490,7 @@
       <alignment readingOrder="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment readingOrder="1"/>
     </xf>
@@ -496,16 +505,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -525,15 +524,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -574,50 +564,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
@@ -649,38 +654,41 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment readingOrder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1226,8 +1234,8 @@
   <sheetPr codeName="Arkusz1"/>
   <dimension ref="A1:IV24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1243,46 +1251,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="27" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="36"/>
-      <c r="AF1" s="36"/>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="36"/>
-      <c r="AI1" s="36"/>
-      <c r="AJ1" s="36"/>
-      <c r="AK1" s="36"/>
-      <c r="AL1" s="36"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="63"/>
+      <c r="X1" s="63"/>
+      <c r="Y1" s="63"/>
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="63"/>
+      <c r="AB1" s="63"/>
+      <c r="AC1" s="64"/>
+      <c r="AD1" s="64"/>
+      <c r="AE1" s="64"/>
+      <c r="AF1" s="64"/>
+      <c r="AG1" s="64"/>
+      <c r="AH1" s="64"/>
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="65"/>
+      <c r="AK1" s="65"/>
+      <c r="AL1" s="65"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
@@ -1503,52 +1511,52 @@
       <c r="IV1" s="1"/>
     </row>
     <row r="2" spans="1:256" ht="9.75" customHeight="1">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="37" t="s">
-        <v>30</v>
+      <c r="A2" s="61"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="66" t="s">
+        <v>29</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37" t="s">
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="37" t="s">
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="66"/>
+      <c r="X2" s="66"/>
+      <c r="Y2" s="66"/>
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
+      <c r="AC2" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="37"/>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="37" t="s">
+      <c r="AD2" s="66"/>
+      <c r="AE2" s="66"/>
+      <c r="AF2" s="66"/>
+      <c r="AG2" s="66"/>
+      <c r="AH2" s="66"/>
+      <c r="AI2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="AJ2" s="37"/>
-      <c r="AK2" s="37"/>
-      <c r="AL2" s="37"/>
+      <c r="AJ2" s="66"/>
+      <c r="AK2" s="66"/>
+      <c r="AL2" s="66"/>
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
@@ -1769,48 +1777,48 @@
       <c r="IV2" s="1"/>
     </row>
     <row r="3" spans="1:256" ht="18" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38" t="s">
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="38"/>
-      <c r="S3" s="38"/>
-      <c r="T3" s="38"/>
-      <c r="U3" s="38"/>
-      <c r="V3" s="38"/>
-      <c r="W3" s="38"/>
-      <c r="X3" s="38"/>
-      <c r="Y3" s="38"/>
-      <c r="Z3" s="38"/>
-      <c r="AA3" s="38"/>
-      <c r="AB3" s="38"/>
-      <c r="AC3" s="38"/>
-      <c r="AD3" s="38"/>
-      <c r="AE3" s="38"/>
-      <c r="AF3" s="38"/>
-      <c r="AG3" s="38"/>
-      <c r="AH3" s="38"/>
-      <c r="AI3" s="38"/>
-      <c r="AJ3" s="38"/>
-      <c r="AK3" s="38"/>
-      <c r="AL3" s="38"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="57"/>
+      <c r="T3" s="57"/>
+      <c r="U3" s="57"/>
+      <c r="V3" s="57"/>
+      <c r="W3" s="57"/>
+      <c r="X3" s="57"/>
+      <c r="Y3" s="57"/>
+      <c r="Z3" s="57"/>
+      <c r="AA3" s="57"/>
+      <c r="AB3" s="57"/>
+      <c r="AC3" s="57"/>
+      <c r="AD3" s="57"/>
+      <c r="AE3" s="57"/>
+      <c r="AF3" s="57"/>
+      <c r="AG3" s="57"/>
+      <c r="AH3" s="57"/>
+      <c r="AI3" s="57"/>
+      <c r="AJ3" s="57"/>
+      <c r="AK3" s="57"/>
+      <c r="AL3" s="57"/>
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
@@ -2031,52 +2039,52 @@
       <c r="IV3" s="1"/>
     </row>
     <row r="4" spans="1:256" ht="14.85" customHeight="1">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="40" t="s">
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="40"/>
-      <c r="S4" s="40"/>
-      <c r="T4" s="40"/>
-      <c r="U4" s="40"/>
-      <c r="V4" s="40"/>
-      <c r="W4" s="40"/>
-      <c r="X4" s="40"/>
-      <c r="Y4" s="40"/>
-      <c r="Z4" s="40"/>
-      <c r="AA4" s="40"/>
-      <c r="AB4" s="40"/>
-      <c r="AC4" s="40"/>
-      <c r="AD4" s="40"/>
-      <c r="AE4" s="40"/>
-      <c r="AF4" s="40"/>
-      <c r="AG4" s="40"/>
-      <c r="AH4" s="40"/>
-      <c r="AI4" s="40" t="s">
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
+      <c r="Y4" s="59"/>
+      <c r="Z4" s="59"/>
+      <c r="AA4" s="59"/>
+      <c r="AB4" s="59"/>
+      <c r="AC4" s="59"/>
+      <c r="AD4" s="59"/>
+      <c r="AE4" s="59"/>
+      <c r="AF4" s="59"/>
+      <c r="AG4" s="59"/>
+      <c r="AH4" s="59"/>
+      <c r="AI4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="AJ4" s="41" t="s">
+      <c r="AJ4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="AK4" s="41"/>
-      <c r="AL4" s="41" t="s">
+      <c r="AK4" s="60"/>
+      <c r="AL4" s="60" t="s">
         <v>10</v>
       </c>
       <c r="AM4" s="2"/>
@@ -2299,44 +2307,44 @@
       <c r="IV4" s="2"/>
     </row>
     <row r="5" spans="1:256" s="4" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="32"/>
-      <c r="S5" s="32"/>
-      <c r="T5" s="32"/>
-      <c r="U5" s="32"/>
-      <c r="V5" s="32"/>
-      <c r="W5" s="32"/>
-      <c r="X5" s="32"/>
-      <c r="Y5" s="32"/>
-      <c r="Z5" s="32"/>
-      <c r="AA5" s="32"/>
-      <c r="AB5" s="32"/>
-      <c r="AC5" s="32"/>
-      <c r="AD5" s="32"/>
-      <c r="AE5" s="32"/>
-      <c r="AF5" s="32"/>
-      <c r="AG5" s="32"/>
-      <c r="AH5" s="32"/>
-      <c r="AI5" s="40"/>
-      <c r="AJ5" s="41"/>
-      <c r="AK5" s="41"/>
-      <c r="AL5" s="41"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="25"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="25"/>
+      <c r="AB5" s="25"/>
+      <c r="AC5" s="25"/>
+      <c r="AD5" s="25"/>
+      <c r="AE5" s="25"/>
+      <c r="AF5" s="25"/>
+      <c r="AG5" s="25"/>
+      <c r="AH5" s="25"/>
+      <c r="AI5" s="59"/>
+      <c r="AJ5" s="60"/>
+      <c r="AK5" s="60"/>
+      <c r="AL5" s="60"/>
       <c r="AM5" s="3"/>
       <c r="AN5" s="3"/>
       <c r="AO5" s="3"/>
@@ -2557,48 +2565,48 @@
       <c r="IV5" s="3"/>
     </row>
     <row r="6" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A6" s="42" t="s">
-        <v>31</v>
+      <c r="A6" s="31" t="s">
+        <v>30</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="29"/>
-      <c r="T6" s="29"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="29"/>
-      <c r="W6" s="29"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="29"/>
-      <c r="Z6" s="29"/>
-      <c r="AA6" s="29"/>
-      <c r="AB6" s="29"/>
-      <c r="AC6" s="29"/>
-      <c r="AD6" s="29"/>
-      <c r="AE6" s="29"/>
-      <c r="AF6" s="29"/>
-      <c r="AG6" s="29"/>
-      <c r="AH6" s="29"/>
-      <c r="AI6" s="11"/>
-      <c r="AJ6" s="44" t="s">
+      <c r="B6" s="31"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="22"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="22"/>
+      <c r="Z6" s="22"/>
+      <c r="AA6" s="22"/>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="22"/>
+      <c r="AE6" s="22"/>
+      <c r="AF6" s="22"/>
+      <c r="AG6" s="22"/>
+      <c r="AH6" s="22"/>
+      <c r="AI6" s="7"/>
+      <c r="AJ6" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="AK6" s="44"/>
-      <c r="AL6" s="5"/>
+      <c r="AK6" s="36"/>
+      <c r="AL6" s="26"/>
       <c r="AM6" s="1"/>
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
@@ -2819,46 +2827,46 @@
       <c r="IV6" s="1"/>
     </row>
     <row r="7" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="30"/>
-      <c r="V7" s="30"/>
-      <c r="W7" s="30"/>
-      <c r="X7" s="30"/>
-      <c r="Y7" s="30"/>
-      <c r="Z7" s="30"/>
-      <c r="AA7" s="30"/>
-      <c r="AB7" s="30"/>
-      <c r="AC7" s="30"/>
-      <c r="AD7" s="30"/>
-      <c r="AE7" s="30"/>
-      <c r="AF7" s="30"/>
-      <c r="AG7" s="30"/>
-      <c r="AH7" s="30"/>
-      <c r="AI7" s="11"/>
-      <c r="AJ7" s="45"/>
-      <c r="AK7" s="45"/>
-      <c r="AL7" s="6"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+      <c r="X7" s="23"/>
+      <c r="Y7" s="23"/>
+      <c r="Z7" s="23"/>
+      <c r="AA7" s="23"/>
+      <c r="AB7" s="23"/>
+      <c r="AC7" s="23"/>
+      <c r="AD7" s="23"/>
+      <c r="AE7" s="23"/>
+      <c r="AF7" s="23"/>
+      <c r="AG7" s="23"/>
+      <c r="AH7" s="23"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="32"/>
+      <c r="AK7" s="32"/>
+      <c r="AL7" s="26"/>
       <c r="AM7" s="1"/>
       <c r="AN7" s="1"/>
       <c r="AO7" s="1"/>
@@ -3079,46 +3087,46 @@
       <c r="IV7" s="1"/>
     </row>
     <row r="8" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
-      <c r="T8" s="31"/>
-      <c r="U8" s="31"/>
-      <c r="V8" s="31"/>
-      <c r="W8" s="31"/>
-      <c r="X8" s="31"/>
-      <c r="Y8" s="31"/>
-      <c r="Z8" s="31"/>
-      <c r="AA8" s="31"/>
-      <c r="AB8" s="31"/>
-      <c r="AC8" s="31"/>
-      <c r="AD8" s="31"/>
-      <c r="AE8" s="31"/>
-      <c r="AF8" s="31"/>
-      <c r="AG8" s="31"/>
-      <c r="AH8" s="31"/>
-      <c r="AI8" s="11"/>
-      <c r="AJ8" s="44" t="s">
+      <c r="A8" s="56"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="24"/>
+      <c r="Z8" s="24"/>
+      <c r="AA8" s="24"/>
+      <c r="AB8" s="24"/>
+      <c r="AC8" s="24"/>
+      <c r="AD8" s="24"/>
+      <c r="AE8" s="24"/>
+      <c r="AF8" s="24"/>
+      <c r="AG8" s="24"/>
+      <c r="AH8" s="24"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="AK8" s="44"/>
-      <c r="AL8" s="6"/>
+      <c r="AK8" s="36"/>
+      <c r="AL8" s="26"/>
       <c r="AM8" s="1"/>
       <c r="AN8" s="1"/>
       <c r="AO8" s="1"/>
@@ -3339,44 +3347,44 @@
       <c r="IV8" s="1"/>
     </row>
     <row r="9" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A9" s="47"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="20"/>
-      <c r="U9" s="20"/>
-      <c r="V9" s="20"/>
-      <c r="W9" s="20"/>
-      <c r="X9" s="20"/>
-      <c r="Y9" s="20"/>
-      <c r="Z9" s="20"/>
-      <c r="AA9" s="20"/>
-      <c r="AB9" s="20"/>
-      <c r="AC9" s="20"/>
-      <c r="AD9" s="20"/>
-      <c r="AE9" s="20"/>
-      <c r="AF9" s="20"/>
-      <c r="AG9" s="20"/>
-      <c r="AH9" s="20"/>
-      <c r="AI9" s="10"/>
-      <c r="AJ9" s="45"/>
-      <c r="AK9" s="45"/>
-      <c r="AL9" s="7"/>
+      <c r="A9" s="45"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="13"/>
+      <c r="AB9" s="13"/>
+      <c r="AC9" s="13"/>
+      <c r="AD9" s="13"/>
+      <c r="AE9" s="13"/>
+      <c r="AF9" s="13"/>
+      <c r="AG9" s="13"/>
+      <c r="AH9" s="13"/>
+      <c r="AI9" s="6"/>
+      <c r="AJ9" s="32"/>
+      <c r="AK9" s="32"/>
+      <c r="AL9" s="27"/>
       <c r="AM9" s="1"/>
       <c r="AN9" s="1"/>
       <c r="AO9" s="1"/>
@@ -3597,44 +3605,44 @@
       <c r="IV9" s="1"/>
     </row>
     <row r="10" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A10" s="48"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="24"/>
-      <c r="S10" s="24"/>
-      <c r="T10" s="24"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="24"/>
-      <c r="X10" s="24"/>
-      <c r="Y10" s="24"/>
-      <c r="Z10" s="24"/>
-      <c r="AA10" s="24"/>
-      <c r="AB10" s="24"/>
-      <c r="AC10" s="24"/>
-      <c r="AD10" s="24"/>
-      <c r="AE10" s="24"/>
-      <c r="AF10" s="24"/>
-      <c r="AG10" s="24"/>
-      <c r="AH10" s="24"/>
-      <c r="AI10" s="10"/>
-      <c r="AJ10" s="45"/>
-      <c r="AK10" s="45"/>
-      <c r="AL10" s="5"/>
+      <c r="A10" s="46"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="17"/>
+      <c r="AA10" s="17"/>
+      <c r="AB10" s="17"/>
+      <c r="AC10" s="17"/>
+      <c r="AD10" s="17"/>
+      <c r="AE10" s="17"/>
+      <c r="AF10" s="17"/>
+      <c r="AG10" s="17"/>
+      <c r="AH10" s="17"/>
+      <c r="AI10" s="6"/>
+      <c r="AJ10" s="32"/>
+      <c r="AK10" s="32"/>
+      <c r="AL10" s="26"/>
       <c r="AM10" s="1"/>
       <c r="AN10" s="1"/>
       <c r="AO10" s="1"/>
@@ -3855,46 +3863,46 @@
       <c r="IV10" s="1"/>
     </row>
     <row r="11" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A11" s="51"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="54"/>
-      <c r="M11" s="54"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="54"/>
-      <c r="P11" s="54"/>
-      <c r="Q11" s="54"/>
-      <c r="R11" s="54"/>
-      <c r="S11" s="54"/>
-      <c r="T11" s="54"/>
-      <c r="U11" s="54"/>
-      <c r="V11" s="54"/>
-      <c r="W11" s="54"/>
-      <c r="X11" s="54"/>
-      <c r="Y11" s="54"/>
-      <c r="Z11" s="54"/>
-      <c r="AA11" s="54"/>
-      <c r="AB11" s="54"/>
-      <c r="AC11" s="54"/>
-      <c r="AD11" s="54"/>
-      <c r="AE11" s="54"/>
-      <c r="AF11" s="54"/>
-      <c r="AG11" s="54"/>
-      <c r="AH11" s="55"/>
-      <c r="AI11" s="19"/>
-      <c r="AJ11" s="56" t="s">
+      <c r="A11" s="49"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="52"/>
+      <c r="P11" s="52"/>
+      <c r="Q11" s="52"/>
+      <c r="R11" s="52"/>
+      <c r="S11" s="52"/>
+      <c r="T11" s="52"/>
+      <c r="U11" s="52"/>
+      <c r="V11" s="52"/>
+      <c r="W11" s="52"/>
+      <c r="X11" s="52"/>
+      <c r="Y11" s="52"/>
+      <c r="Z11" s="52"/>
+      <c r="AA11" s="52"/>
+      <c r="AB11" s="52"/>
+      <c r="AC11" s="52"/>
+      <c r="AD11" s="52"/>
+      <c r="AE11" s="52"/>
+      <c r="AF11" s="52"/>
+      <c r="AG11" s="52"/>
+      <c r="AH11" s="53"/>
+      <c r="AI11" s="12"/>
+      <c r="AJ11" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="AK11" s="56"/>
-      <c r="AL11" s="16"/>
+      <c r="AK11" s="54"/>
+      <c r="AL11" s="28"/>
       <c r="AM11" s="1"/>
       <c r="AN11" s="1"/>
       <c r="AO11" s="1"/>
@@ -4115,48 +4123,48 @@
       <c r="IV11" s="1"/>
     </row>
     <row r="12" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26"/>
-      <c r="R12" s="26"/>
-      <c r="S12" s="26"/>
-      <c r="T12" s="26"/>
-      <c r="U12" s="26"/>
-      <c r="V12" s="26"/>
-      <c r="W12" s="26"/>
-      <c r="X12" s="26"/>
-      <c r="Y12" s="26"/>
-      <c r="Z12" s="26"/>
-      <c r="AA12" s="26"/>
-      <c r="AB12" s="26"/>
-      <c r="AC12" s="26"/>
-      <c r="AD12" s="26"/>
-      <c r="AE12" s="26"/>
-      <c r="AF12" s="26"/>
-      <c r="AG12" s="26"/>
-      <c r="AH12" s="26"/>
-      <c r="AI12" s="15"/>
-      <c r="AJ12" s="58" t="s">
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
+      <c r="X12" s="19"/>
+      <c r="Y12" s="19"/>
+      <c r="Z12" s="19"/>
+      <c r="AA12" s="19"/>
+      <c r="AB12" s="19"/>
+      <c r="AC12" s="19"/>
+      <c r="AD12" s="19"/>
+      <c r="AE12" s="19"/>
+      <c r="AF12" s="19"/>
+      <c r="AG12" s="19"/>
+      <c r="AH12" s="19"/>
+      <c r="AI12" s="11"/>
+      <c r="AJ12" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="AK12" s="59"/>
-      <c r="AL12" s="18"/>
+      <c r="AK12" s="40"/>
+      <c r="AL12" s="29"/>
       <c r="AM12" s="1"/>
       <c r="AN12" s="1"/>
       <c r="AO12" s="1"/>
@@ -4377,50 +4385,50 @@
       <c r="IV12" s="1"/>
     </row>
     <row r="13" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="62" t="s">
+      <c r="B13" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="27"/>
-      <c r="T13" s="27"/>
-      <c r="U13" s="27"/>
-      <c r="V13" s="27"/>
-      <c r="W13" s="27"/>
-      <c r="X13" s="27"/>
-      <c r="Y13" s="27"/>
-      <c r="Z13" s="27"/>
-      <c r="AA13" s="27"/>
-      <c r="AB13" s="27"/>
-      <c r="AC13" s="27"/>
-      <c r="AD13" s="27"/>
-      <c r="AE13" s="27"/>
-      <c r="AF13" s="27"/>
-      <c r="AG13" s="27"/>
-      <c r="AH13" s="27"/>
-      <c r="AI13" s="14"/>
-      <c r="AJ13" s="63" t="s">
+      <c r="C13" s="43"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="20"/>
+      <c r="V13" s="20"/>
+      <c r="W13" s="20"/>
+      <c r="X13" s="20"/>
+      <c r="Y13" s="20"/>
+      <c r="Z13" s="20"/>
+      <c r="AA13" s="20"/>
+      <c r="AB13" s="20"/>
+      <c r="AC13" s="20"/>
+      <c r="AD13" s="20"/>
+      <c r="AE13" s="20"/>
+      <c r="AF13" s="20"/>
+      <c r="AG13" s="20"/>
+      <c r="AH13" s="20"/>
+      <c r="AI13" s="10"/>
+      <c r="AJ13" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="AK13" s="63"/>
-      <c r="AL13" s="17"/>
+      <c r="AK13" s="44"/>
+      <c r="AL13" s="30"/>
       <c r="AM13" s="1"/>
       <c r="AN13" s="1"/>
       <c r="AO13" s="1"/>
@@ -4641,48 +4649,48 @@
       <c r="IV13" s="1"/>
     </row>
     <row r="14" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A14" s="61"/>
-      <c r="B14" s="44" t="s">
+      <c r="A14" s="42"/>
+      <c r="B14" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="10"/>
-      <c r="Y14" s="10"/>
-      <c r="Z14" s="10"/>
-      <c r="AA14" s="10"/>
-      <c r="AB14" s="10"/>
-      <c r="AC14" s="12"/>
-      <c r="AD14" s="10"/>
-      <c r="AE14" s="10"/>
-      <c r="AF14" s="10"/>
-      <c r="AG14" s="10"/>
-      <c r="AH14" s="10"/>
-      <c r="AI14" s="10"/>
-      <c r="AJ14" s="44" t="s">
+      <c r="C14" s="36"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="6"/>
+      <c r="AC14" s="8"/>
+      <c r="AD14" s="6"/>
+      <c r="AE14" s="6"/>
+      <c r="AF14" s="6"/>
+      <c r="AG14" s="6"/>
+      <c r="AH14" s="6"/>
+      <c r="AI14" s="6"/>
+      <c r="AJ14" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="AK14" s="44"/>
-      <c r="AL14" s="8"/>
+      <c r="AK14" s="36"/>
+      <c r="AL14" s="26"/>
       <c r="AM14" s="1"/>
       <c r="AN14" s="1"/>
       <c r="AO14" s="1"/>
@@ -4903,48 +4911,48 @@
       <c r="IV14" s="1"/>
     </row>
     <row r="15" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A15" s="61"/>
-      <c r="B15" s="44" t="s">
+      <c r="A15" s="42"/>
+      <c r="B15" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
-      <c r="V15" s="10"/>
-      <c r="W15" s="10"/>
-      <c r="X15" s="10"/>
-      <c r="Y15" s="10"/>
-      <c r="Z15" s="10"/>
-      <c r="AA15" s="10"/>
-      <c r="AB15" s="10"/>
-      <c r="AC15" s="12"/>
-      <c r="AD15" s="12"/>
-      <c r="AE15" s="10"/>
-      <c r="AF15" s="10"/>
-      <c r="AG15" s="10"/>
-      <c r="AH15" s="10"/>
-      <c r="AI15" s="10"/>
-      <c r="AJ15" s="44" t="s">
+      <c r="C15" s="36"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="8"/>
+      <c r="AD15" s="8"/>
+      <c r="AE15" s="6"/>
+      <c r="AF15" s="6"/>
+      <c r="AG15" s="6"/>
+      <c r="AH15" s="6"/>
+      <c r="AI15" s="6"/>
+      <c r="AJ15" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="AK15" s="44"/>
-      <c r="AL15" s="5"/>
+      <c r="AK15" s="36"/>
+      <c r="AL15" s="26"/>
       <c r="AM15" s="1"/>
       <c r="AN15" s="1"/>
       <c r="AO15" s="1"/>
@@ -5165,48 +5173,48 @@
       <c r="IV15" s="1"/>
     </row>
     <row r="16" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A16" s="61"/>
-      <c r="B16" s="44" t="s">
+      <c r="A16" s="42"/>
+      <c r="B16" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10"/>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="10"/>
-      <c r="AA16" s="10"/>
-      <c r="AB16" s="10"/>
-      <c r="AC16" s="12"/>
-      <c r="AD16" s="12"/>
-      <c r="AE16" s="10"/>
-      <c r="AF16" s="10"/>
-      <c r="AG16" s="10"/>
-      <c r="AH16" s="10"/>
-      <c r="AI16" s="10"/>
-      <c r="AJ16" s="44" t="s">
+      <c r="C16" s="36"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="8"/>
+      <c r="AD16" s="8"/>
+      <c r="AE16" s="6"/>
+      <c r="AF16" s="6"/>
+      <c r="AG16" s="6"/>
+      <c r="AH16" s="6"/>
+      <c r="AI16" s="6"/>
+      <c r="AJ16" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="AK16" s="44"/>
-      <c r="AL16" s="5"/>
+      <c r="AK16" s="36"/>
+      <c r="AL16" s="26"/>
       <c r="AM16" s="1"/>
       <c r="AN16" s="1"/>
       <c r="AO16" s="1"/>
@@ -5427,48 +5435,48 @@
       <c r="IV16" s="1"/>
     </row>
     <row r="17" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A17" s="61"/>
-      <c r="B17" s="44" t="s">
+      <c r="A17" s="42"/>
+      <c r="B17" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="10"/>
-      <c r="Y17" s="10"/>
-      <c r="Z17" s="10"/>
-      <c r="AA17" s="10"/>
-      <c r="AB17" s="10"/>
-      <c r="AC17" s="12"/>
-      <c r="AD17" s="10"/>
-      <c r="AE17" s="10"/>
-      <c r="AF17" s="10"/>
-      <c r="AG17" s="10"/>
-      <c r="AH17" s="10"/>
-      <c r="AI17" s="10"/>
-      <c r="AJ17" s="44" t="s">
+      <c r="C17" s="36"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="8"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="6"/>
+      <c r="AF17" s="6"/>
+      <c r="AG17" s="6"/>
+      <c r="AH17" s="6"/>
+      <c r="AI17" s="6"/>
+      <c r="AJ17" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="AK17" s="44"/>
-      <c r="AL17" s="5"/>
+      <c r="AK17" s="36"/>
+      <c r="AL17" s="26"/>
       <c r="AM17" s="1"/>
       <c r="AN17" s="1"/>
       <c r="AO17" s="1"/>
@@ -5689,48 +5697,48 @@
       <c r="IV17" s="1"/>
     </row>
     <row r="18" spans="1:256" ht="24.75" customHeight="1">
-      <c r="A18" s="61"/>
-      <c r="B18" s="42" t="s">
+      <c r="A18" s="42"/>
+      <c r="B18" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="12"/>
-      <c r="W18" s="12"/>
-      <c r="X18" s="10"/>
-      <c r="Y18" s="10"/>
-      <c r="Z18" s="10"/>
-      <c r="AA18" s="10"/>
-      <c r="AB18" s="10"/>
-      <c r="AC18" s="10"/>
-      <c r="AD18" s="10"/>
-      <c r="AE18" s="10"/>
-      <c r="AF18" s="10"/>
-      <c r="AG18" s="10"/>
-      <c r="AH18" s="10"/>
-      <c r="AI18" s="10"/>
-      <c r="AJ18" s="42" t="s">
+      <c r="C18" s="31"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="6"/>
+      <c r="AD18" s="6"/>
+      <c r="AE18" s="6"/>
+      <c r="AF18" s="6"/>
+      <c r="AG18" s="6"/>
+      <c r="AH18" s="6"/>
+      <c r="AI18" s="6"/>
+      <c r="AJ18" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AK18" s="42"/>
-      <c r="AL18" s="5"/>
+      <c r="AK18" s="31"/>
+      <c r="AL18" s="26"/>
       <c r="AM18" s="1"/>
       <c r="AN18" s="1"/>
       <c r="AO18" s="1"/>
@@ -5951,48 +5959,48 @@
       <c r="IV18" s="1"/>
     </row>
     <row r="19" spans="1:256" ht="24.75" customHeight="1">
-      <c r="A19" s="61"/>
-      <c r="B19" s="42" t="s">
+      <c r="A19" s="42"/>
+      <c r="B19" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
-      <c r="V19" s="12"/>
-      <c r="W19" s="12"/>
-      <c r="X19" s="10"/>
-      <c r="Y19" s="10"/>
-      <c r="Z19" s="10"/>
-      <c r="AA19" s="10"/>
-      <c r="AB19" s="10"/>
-      <c r="AC19" s="10"/>
-      <c r="AD19" s="10"/>
-      <c r="AE19" s="10"/>
-      <c r="AF19" s="10"/>
-      <c r="AG19" s="10"/>
-      <c r="AH19" s="10"/>
-      <c r="AI19" s="10"/>
-      <c r="AJ19" s="42" t="s">
+      <c r="C19" s="31"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="6"/>
+      <c r="AA19" s="6"/>
+      <c r="AB19" s="6"/>
+      <c r="AC19" s="6"/>
+      <c r="AD19" s="6"/>
+      <c r="AE19" s="6"/>
+      <c r="AF19" s="6"/>
+      <c r="AG19" s="6"/>
+      <c r="AH19" s="6"/>
+      <c r="AI19" s="6"/>
+      <c r="AJ19" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="AK19" s="42"/>
-      <c r="AL19" s="5"/>
+      <c r="AK19" s="31"/>
+      <c r="AL19" s="26"/>
       <c r="AM19" s="1"/>
       <c r="AN19" s="1"/>
       <c r="AO19" s="1"/>
@@ -6213,46 +6221,46 @@
       <c r="IV19" s="1"/>
     </row>
     <row r="20" spans="1:256" ht="24.75" customHeight="1">
-      <c r="A20" s="61"/>
-      <c r="B20" s="66" t="s">
+      <c r="A20" s="42"/>
+      <c r="B20" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="66"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="10"/>
-      <c r="W20" s="10"/>
-      <c r="X20" s="10"/>
-      <c r="Y20" s="10"/>
-      <c r="Z20" s="10"/>
-      <c r="AA20" s="10"/>
-      <c r="AB20" s="10"/>
-      <c r="AC20" s="10"/>
-      <c r="AD20" s="10"/>
-      <c r="AE20" s="10"/>
-      <c r="AF20" s="10"/>
-      <c r="AG20" s="10"/>
-      <c r="AH20" s="10"/>
-      <c r="AI20" s="10"/>
-      <c r="AJ20" s="45"/>
-      <c r="AK20" s="45"/>
-      <c r="AL20" s="5"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="6"/>
+      <c r="AE20" s="6"/>
+      <c r="AF20" s="6"/>
+      <c r="AG20" s="6"/>
+      <c r="AH20" s="6"/>
+      <c r="AI20" s="6"/>
+      <c r="AJ20" s="32"/>
+      <c r="AK20" s="32"/>
+      <c r="AL20" s="26"/>
       <c r="AM20" s="1"/>
       <c r="AN20" s="1"/>
       <c r="AO20" s="1"/>
@@ -6473,46 +6481,46 @@
       <c r="IV20" s="1"/>
     </row>
     <row r="21" spans="1:256" ht="17.25" customHeight="1">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="67"/>
-      <c r="K21" s="67"/>
-      <c r="L21" s="67"/>
-      <c r="M21" s="67"/>
-      <c r="N21" s="67"/>
-      <c r="O21" s="67"/>
-      <c r="P21" s="67"/>
-      <c r="Q21" s="67"/>
-      <c r="R21" s="67"/>
-      <c r="S21" s="67"/>
-      <c r="T21" s="67"/>
-      <c r="U21" s="67"/>
-      <c r="V21" s="67"/>
-      <c r="W21" s="67"/>
-      <c r="X21" s="67"/>
-      <c r="Y21" s="67"/>
-      <c r="Z21" s="67"/>
-      <c r="AA21" s="67"/>
-      <c r="AB21" s="67"/>
-      <c r="AC21" s="67"/>
-      <c r="AD21" s="67"/>
-      <c r="AE21" s="67"/>
-      <c r="AF21" s="67"/>
-      <c r="AG21" s="67"/>
-      <c r="AH21" s="67"/>
-      <c r="AI21" s="13"/>
-      <c r="AJ21" s="45"/>
-      <c r="AK21" s="45"/>
-      <c r="AL21" s="5"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="37"/>
+      <c r="R21" s="37"/>
+      <c r="S21" s="37"/>
+      <c r="T21" s="37"/>
+      <c r="U21" s="37"/>
+      <c r="V21" s="37"/>
+      <c r="W21" s="37"/>
+      <c r="X21" s="37"/>
+      <c r="Y21" s="37"/>
+      <c r="Z21" s="37"/>
+      <c r="AA21" s="37"/>
+      <c r="AB21" s="37"/>
+      <c r="AC21" s="37"/>
+      <c r="AD21" s="37"/>
+      <c r="AE21" s="37"/>
+      <c r="AF21" s="37"/>
+      <c r="AG21" s="37"/>
+      <c r="AH21" s="37"/>
+      <c r="AI21" s="9"/>
+      <c r="AJ21" s="32"/>
+      <c r="AK21" s="32"/>
+      <c r="AL21" s="26"/>
       <c r="AM21" s="1"/>
       <c r="AN21" s="1"/>
       <c r="AO21" s="1"/>
@@ -6733,44 +6741,44 @@
       <c r="IV21" s="1"/>
     </row>
     <row r="22" spans="1:256" ht="15.75" customHeight="1">
-      <c r="A22" s="44"/>
-      <c r="B22" s="44"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="67"/>
-      <c r="J22" s="67"/>
-      <c r="K22" s="67"/>
-      <c r="L22" s="67"/>
-      <c r="M22" s="67"/>
-      <c r="N22" s="67"/>
-      <c r="O22" s="67"/>
-      <c r="P22" s="67"/>
-      <c r="Q22" s="67"/>
-      <c r="R22" s="67"/>
-      <c r="S22" s="67"/>
-      <c r="T22" s="67"/>
-      <c r="U22" s="67"/>
-      <c r="V22" s="67"/>
-      <c r="W22" s="67"/>
-      <c r="X22" s="67"/>
-      <c r="Y22" s="67"/>
-      <c r="Z22" s="67"/>
-      <c r="AA22" s="67"/>
-      <c r="AB22" s="67"/>
-      <c r="AC22" s="67"/>
-      <c r="AD22" s="67"/>
-      <c r="AE22" s="67"/>
-      <c r="AF22" s="67"/>
-      <c r="AG22" s="67"/>
-      <c r="AH22" s="67"/>
-      <c r="AI22" s="10"/>
-      <c r="AJ22" s="45"/>
-      <c r="AK22" s="45"/>
-      <c r="AL22" s="5"/>
+      <c r="A22" s="36"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="37"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="37"/>
+      <c r="U22" s="37"/>
+      <c r="V22" s="37"/>
+      <c r="W22" s="37"/>
+      <c r="X22" s="37"/>
+      <c r="Y22" s="37"/>
+      <c r="Z22" s="37"/>
+      <c r="AA22" s="37"/>
+      <c r="AB22" s="37"/>
+      <c r="AC22" s="37"/>
+      <c r="AD22" s="37"/>
+      <c r="AE22" s="37"/>
+      <c r="AF22" s="37"/>
+      <c r="AG22" s="37"/>
+      <c r="AH22" s="37"/>
+      <c r="AI22" s="6"/>
+      <c r="AJ22" s="32"/>
+      <c r="AK22" s="32"/>
+      <c r="AL22" s="26"/>
       <c r="AM22" s="1"/>
       <c r="AN22" s="1"/>
       <c r="AO22" s="1"/>
@@ -6991,46 +6999,46 @@
       <c r="IV22" s="1"/>
     </row>
     <row r="23" spans="1:256" ht="18.75" customHeight="1">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10"/>
-      <c r="T23" s="10"/>
-      <c r="U23" s="10"/>
-      <c r="V23" s="10"/>
-      <c r="W23" s="10"/>
-      <c r="X23" s="10"/>
-      <c r="Y23" s="10"/>
-      <c r="Z23" s="10"/>
-      <c r="AA23" s="10"/>
-      <c r="AB23" s="10"/>
-      <c r="AC23" s="10"/>
-      <c r="AD23" s="10"/>
-      <c r="AE23" s="10"/>
-      <c r="AF23" s="10"/>
-      <c r="AG23" s="10"/>
-      <c r="AH23" s="10"/>
-      <c r="AI23" s="10"/>
-      <c r="AJ23" s="45"/>
-      <c r="AK23" s="45"/>
-      <c r="AL23" s="5"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+      <c r="Y23" s="6"/>
+      <c r="Z23" s="6"/>
+      <c r="AA23" s="6"/>
+      <c r="AB23" s="6"/>
+      <c r="AC23" s="6"/>
+      <c r="AD23" s="6"/>
+      <c r="AE23" s="6"/>
+      <c r="AF23" s="6"/>
+      <c r="AG23" s="6"/>
+      <c r="AH23" s="6"/>
+      <c r="AI23" s="6"/>
+      <c r="AJ23" s="32"/>
+      <c r="AK23" s="32"/>
+      <c r="AL23" s="26"/>
       <c r="AM23" s="1"/>
       <c r="AN23" s="1"/>
       <c r="AO23" s="1"/>
@@ -7251,48 +7259,48 @@
       <c r="IV23" s="1"/>
     </row>
     <row r="24" spans="1:256" ht="23.4" customHeight="1">
-      <c r="A24" s="64" t="s">
-        <v>29</v>
+      <c r="A24" s="33" t="s">
+        <v>31</v>
       </c>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="64"/>
-      <c r="G24" s="64"/>
-      <c r="H24" s="64"/>
-      <c r="I24" s="64"/>
-      <c r="J24" s="64"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="64"/>
-      <c r="M24" s="64"/>
-      <c r="N24" s="64"/>
-      <c r="O24" s="64"/>
-      <c r="P24" s="64"/>
-      <c r="Q24" s="64"/>
-      <c r="R24" s="64"/>
-      <c r="S24" s="64"/>
-      <c r="T24" s="64"/>
-      <c r="U24" s="64"/>
-      <c r="V24" s="64"/>
-      <c r="W24" s="64"/>
-      <c r="X24" s="64"/>
-      <c r="Y24" s="64"/>
-      <c r="Z24" s="64"/>
-      <c r="AA24" s="64"/>
-      <c r="AB24" s="64"/>
-      <c r="AC24" s="64"/>
-      <c r="AD24" s="64"/>
-      <c r="AE24" s="64"/>
-      <c r="AF24" s="64"/>
-      <c r="AG24" s="64"/>
-      <c r="AH24" s="64"/>
-      <c r="AI24" s="64"/>
-      <c r="AJ24" s="65" t="s">
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="33"/>
+      <c r="P24" s="33"/>
+      <c r="Q24" s="33"/>
+      <c r="R24" s="33"/>
+      <c r="S24" s="33"/>
+      <c r="T24" s="33"/>
+      <c r="U24" s="33"/>
+      <c r="V24" s="33"/>
+      <c r="W24" s="33"/>
+      <c r="X24" s="33"/>
+      <c r="Y24" s="33"/>
+      <c r="Z24" s="33"/>
+      <c r="AA24" s="33"/>
+      <c r="AB24" s="33"/>
+      <c r="AC24" s="33"/>
+      <c r="AD24" s="33"/>
+      <c r="AE24" s="33"/>
+      <c r="AF24" s="33"/>
+      <c r="AG24" s="33"/>
+      <c r="AH24" s="33"/>
+      <c r="AI24" s="33"/>
+      <c r="AJ24" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="AK24" s="65"/>
-      <c r="AL24" s="5"/>
+      <c r="AK24" s="34"/>
+      <c r="AL24" s="26"/>
       <c r="AM24" s="1"/>
       <c r="AN24" s="1"/>
       <c r="AO24" s="1"/>
@@ -7514,17 +7522,35 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="AJ19:AK19"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="AJ23:AK23"/>
-    <mergeCell ref="A24:AI24"/>
-    <mergeCell ref="AJ24:AK24"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="AJ20:AK20"/>
-    <mergeCell ref="A21:C22"/>
-    <mergeCell ref="D21:AH22"/>
-    <mergeCell ref="AJ21:AK21"/>
-    <mergeCell ref="AJ22:AK22"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="M1:AB1"/>
+    <mergeCell ref="AC1:AH1"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="M2:AB2"/>
+    <mergeCell ref="AC2:AH2"/>
+    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="M3:AL3"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="D4:AH4"/>
+    <mergeCell ref="AI4:AI5"/>
+    <mergeCell ref="AJ4:AK5"/>
+    <mergeCell ref="AL4:AL5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="AJ6:AK6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="AJ7:AK7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="AJ8:AK8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="AJ9:AK9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="AJ10:AK10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:AH11"/>
+    <mergeCell ref="AJ11:AK11"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="AJ12:AK12"/>
     <mergeCell ref="A13:A20"/>
@@ -7541,35 +7567,17 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="AJ18:AK18"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="AJ9:AK9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="AJ10:AK10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:AH11"/>
-    <mergeCell ref="AJ11:AK11"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="AJ6:AK6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="AJ7:AK7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="AJ8:AK8"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="M3:AL3"/>
-    <mergeCell ref="A4:C5"/>
-    <mergeCell ref="D4:AH4"/>
-    <mergeCell ref="AI4:AI5"/>
-    <mergeCell ref="AJ4:AK5"/>
-    <mergeCell ref="AL4:AL5"/>
-    <mergeCell ref="A1:F2"/>
-    <mergeCell ref="G1:L1"/>
-    <mergeCell ref="M1:AB1"/>
-    <mergeCell ref="AC1:AH1"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="M2:AB2"/>
-    <mergeCell ref="AC2:AH2"/>
-    <mergeCell ref="AI2:AL2"/>
+    <mergeCell ref="AJ19:AK19"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="AJ23:AK23"/>
+    <mergeCell ref="A24:AI24"/>
+    <mergeCell ref="AJ24:AK24"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="AJ20:AK20"/>
+    <mergeCell ref="A21:C22"/>
+    <mergeCell ref="D21:AH22"/>
+    <mergeCell ref="AJ21:AK21"/>
+    <mergeCell ref="AJ22:AK22"/>
   </mergeCells>
   <conditionalFormatting sqref="D23:AH23">
     <cfRule type="cellIs" dxfId="36" priority="196" operator="equal">

</xml_diff>

<commit_message>
Add list for Days off and unpresence in sehedule model
</commit_message>
<xml_diff>
--- a/GPERP_APP/Resources/Templates/Karta_pracy.xlsx
+++ b/GPERP_APP/Resources/Templates/Karta_pracy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\projekty GitHub\GlassPlant-ERP\GPERP_APP\Resources\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C326F0C-2D2D-4AF0-962D-66C5B1C12EB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFA3C77-7781-449E-933F-31AF76BC1B29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -490,7 +490,7 @@
       <alignment readingOrder="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment readingOrder="1"/>
     </xf>
@@ -580,6 +580,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1234,8 +1237,8 @@
   <sheetPr codeName="Arkusz1"/>
   <dimension ref="A1:IV24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1251,46 +1254,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="27" customHeight="1">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="63"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="63"/>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="63"/>
-      <c r="AB1" s="63"/>
-      <c r="AC1" s="64"/>
-      <c r="AD1" s="64"/>
-      <c r="AE1" s="64"/>
-      <c r="AF1" s="64"/>
-      <c r="AG1" s="64"/>
-      <c r="AH1" s="64"/>
-      <c r="AI1" s="65"/>
-      <c r="AJ1" s="65"/>
-      <c r="AK1" s="65"/>
-      <c r="AL1" s="65"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="64"/>
+      <c r="T1" s="64"/>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="64"/>
+      <c r="X1" s="64"/>
+      <c r="Y1" s="64"/>
+      <c r="Z1" s="64"/>
+      <c r="AA1" s="64"/>
+      <c r="AB1" s="64"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
+      <c r="AE1" s="65"/>
+      <c r="AF1" s="65"/>
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="65"/>
+      <c r="AI1" s="66"/>
+      <c r="AJ1" s="66"/>
+      <c r="AK1" s="66"/>
+      <c r="AL1" s="66"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
@@ -1511,52 +1514,52 @@
       <c r="IV1" s="1"/>
     </row>
     <row r="2" spans="1:256" ht="9.75" customHeight="1">
-      <c r="A2" s="61"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="66" t="s">
+      <c r="A2" s="62"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66" t="s">
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="66"/>
-      <c r="X2" s="66"/>
-      <c r="Y2" s="66"/>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="66"/>
-      <c r="AC2" s="66" t="s">
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="67"/>
+      <c r="T2" s="67"/>
+      <c r="U2" s="67"/>
+      <c r="V2" s="67"/>
+      <c r="W2" s="67"/>
+      <c r="X2" s="67"/>
+      <c r="Y2" s="67"/>
+      <c r="Z2" s="67"/>
+      <c r="AA2" s="67"/>
+      <c r="AB2" s="67"/>
+      <c r="AC2" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
-      <c r="AF2" s="66"/>
-      <c r="AG2" s="66"/>
-      <c r="AH2" s="66"/>
-      <c r="AI2" s="66" t="s">
+      <c r="AD2" s="67"/>
+      <c r="AE2" s="67"/>
+      <c r="AF2" s="67"/>
+      <c r="AG2" s="67"/>
+      <c r="AH2" s="67"/>
+      <c r="AI2" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="AJ2" s="66"/>
-      <c r="AK2" s="66"/>
-      <c r="AL2" s="66"/>
+      <c r="AJ2" s="67"/>
+      <c r="AK2" s="67"/>
+      <c r="AL2" s="67"/>
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
@@ -1777,48 +1780,48 @@
       <c r="IV2" s="1"/>
     </row>
     <row r="3" spans="1:256" ht="18" customHeight="1">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57" t="s">
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="57"/>
-      <c r="T3" s="57"/>
-      <c r="U3" s="57"/>
-      <c r="V3" s="57"/>
-      <c r="W3" s="57"/>
-      <c r="X3" s="57"/>
-      <c r="Y3" s="57"/>
-      <c r="Z3" s="57"/>
-      <c r="AA3" s="57"/>
-      <c r="AB3" s="57"/>
-      <c r="AC3" s="57"/>
-      <c r="AD3" s="57"/>
-      <c r="AE3" s="57"/>
-      <c r="AF3" s="57"/>
-      <c r="AG3" s="57"/>
-      <c r="AH3" s="57"/>
-      <c r="AI3" s="57"/>
-      <c r="AJ3" s="57"/>
-      <c r="AK3" s="57"/>
-      <c r="AL3" s="57"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58"/>
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58"/>
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="58"/>
+      <c r="AC3" s="58"/>
+      <c r="AD3" s="58"/>
+      <c r="AE3" s="58"/>
+      <c r="AF3" s="58"/>
+      <c r="AG3" s="58"/>
+      <c r="AH3" s="58"/>
+      <c r="AI3" s="58"/>
+      <c r="AJ3" s="58"/>
+      <c r="AK3" s="58"/>
+      <c r="AL3" s="58"/>
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
@@ -2039,52 +2042,52 @@
       <c r="IV3" s="1"/>
     </row>
     <row r="4" spans="1:256" ht="14.85" customHeight="1">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="59" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59"/>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="59"/>
-      <c r="T4" s="59"/>
-      <c r="U4" s="59"/>
-      <c r="V4" s="59"/>
-      <c r="W4" s="59"/>
-      <c r="X4" s="59"/>
-      <c r="Y4" s="59"/>
-      <c r="Z4" s="59"/>
-      <c r="AA4" s="59"/>
-      <c r="AB4" s="59"/>
-      <c r="AC4" s="59"/>
-      <c r="AD4" s="59"/>
-      <c r="AE4" s="59"/>
-      <c r="AF4" s="59"/>
-      <c r="AG4" s="59"/>
-      <c r="AH4" s="59"/>
-      <c r="AI4" s="59" t="s">
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="60"/>
+      <c r="R4" s="60"/>
+      <c r="S4" s="60"/>
+      <c r="T4" s="60"/>
+      <c r="U4" s="60"/>
+      <c r="V4" s="60"/>
+      <c r="W4" s="60"/>
+      <c r="X4" s="60"/>
+      <c r="Y4" s="60"/>
+      <c r="Z4" s="60"/>
+      <c r="AA4" s="60"/>
+      <c r="AB4" s="60"/>
+      <c r="AC4" s="60"/>
+      <c r="AD4" s="60"/>
+      <c r="AE4" s="60"/>
+      <c r="AF4" s="60"/>
+      <c r="AG4" s="60"/>
+      <c r="AH4" s="60"/>
+      <c r="AI4" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="AJ4" s="60" t="s">
+      <c r="AJ4" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="AK4" s="60"/>
-      <c r="AL4" s="60" t="s">
+      <c r="AK4" s="61"/>
+      <c r="AL4" s="61" t="s">
         <v>10</v>
       </c>
       <c r="AM4" s="2"/>
@@ -2307,9 +2310,9 @@
       <c r="IV4" s="2"/>
     </row>
     <row r="5" spans="1:256" s="4" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A5" s="58"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="25"/>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
@@ -2341,10 +2344,10 @@
       <c r="AF5" s="25"/>
       <c r="AG5" s="25"/>
       <c r="AH5" s="25"/>
-      <c r="AI5" s="59"/>
-      <c r="AJ5" s="60"/>
-      <c r="AK5" s="60"/>
-      <c r="AL5" s="60"/>
+      <c r="AI5" s="60"/>
+      <c r="AJ5" s="61"/>
+      <c r="AK5" s="61"/>
+      <c r="AL5" s="61"/>
       <c r="AM5" s="3"/>
       <c r="AN5" s="3"/>
       <c r="AO5" s="3"/>
@@ -2565,11 +2568,11 @@
       <c r="IV5" s="3"/>
     </row>
     <row r="6" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="55"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
@@ -2602,11 +2605,11 @@
       <c r="AG6" s="22"/>
       <c r="AH6" s="22"/>
       <c r="AI6" s="7"/>
-      <c r="AJ6" s="36" t="s">
+      <c r="AJ6" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="AK6" s="36"/>
-      <c r="AL6" s="26"/>
+      <c r="AK6" s="37"/>
+      <c r="AL6" s="31"/>
       <c r="AM6" s="1"/>
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
@@ -2827,11 +2830,11 @@
       <c r="IV6" s="1"/>
     </row>
     <row r="7" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
       <c r="F7" s="23"/>
@@ -2864,8 +2867,8 @@
       <c r="AG7" s="23"/>
       <c r="AH7" s="23"/>
       <c r="AI7" s="7"/>
-      <c r="AJ7" s="32"/>
-      <c r="AK7" s="32"/>
+      <c r="AJ7" s="33"/>
+      <c r="AK7" s="33"/>
       <c r="AL7" s="26"/>
       <c r="AM7" s="1"/>
       <c r="AN7" s="1"/>
@@ -3087,9 +3090,9 @@
       <c r="IV7" s="1"/>
     </row>
     <row r="8" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A8" s="56"/>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
       <c r="F8" s="24"/>
@@ -3122,10 +3125,10 @@
       <c r="AG8" s="24"/>
       <c r="AH8" s="24"/>
       <c r="AI8" s="7"/>
-      <c r="AJ8" s="36" t="s">
+      <c r="AJ8" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="AK8" s="36"/>
+      <c r="AK8" s="37"/>
       <c r="AL8" s="26"/>
       <c r="AM8" s="1"/>
       <c r="AN8" s="1"/>
@@ -3347,9 +3350,9 @@
       <c r="IV8" s="1"/>
     </row>
     <row r="9" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A9" s="45"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
+      <c r="A9" s="46"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -3382,8 +3385,8 @@
       <c r="AG9" s="13"/>
       <c r="AH9" s="13"/>
       <c r="AI9" s="6"/>
-      <c r="AJ9" s="32"/>
-      <c r="AK9" s="32"/>
+      <c r="AJ9" s="33"/>
+      <c r="AK9" s="33"/>
       <c r="AL9" s="27"/>
       <c r="AM9" s="1"/>
       <c r="AN9" s="1"/>
@@ -3605,9 +3608,9 @@
       <c r="IV9" s="1"/>
     </row>
     <row r="10" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A10" s="46"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="48"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="15"/>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
@@ -3640,8 +3643,8 @@
       <c r="AG10" s="17"/>
       <c r="AH10" s="17"/>
       <c r="AI10" s="6"/>
-      <c r="AJ10" s="32"/>
-      <c r="AK10" s="32"/>
+      <c r="AJ10" s="33"/>
+      <c r="AK10" s="33"/>
       <c r="AL10" s="26"/>
       <c r="AM10" s="1"/>
       <c r="AN10" s="1"/>
@@ -3863,45 +3866,45 @@
       <c r="IV10" s="1"/>
     </row>
     <row r="11" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A11" s="49"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52"/>
-      <c r="O11" s="52"/>
-      <c r="P11" s="52"/>
-      <c r="Q11" s="52"/>
-      <c r="R11" s="52"/>
-      <c r="S11" s="52"/>
-      <c r="T11" s="52"/>
-      <c r="U11" s="52"/>
-      <c r="V11" s="52"/>
-      <c r="W11" s="52"/>
-      <c r="X11" s="52"/>
-      <c r="Y11" s="52"/>
-      <c r="Z11" s="52"/>
-      <c r="AA11" s="52"/>
-      <c r="AB11" s="52"/>
-      <c r="AC11" s="52"/>
-      <c r="AD11" s="52"/>
-      <c r="AE11" s="52"/>
-      <c r="AF11" s="52"/>
-      <c r="AG11" s="52"/>
-      <c r="AH11" s="53"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="53"/>
+      <c r="O11" s="53"/>
+      <c r="P11" s="53"/>
+      <c r="Q11" s="53"/>
+      <c r="R11" s="53"/>
+      <c r="S11" s="53"/>
+      <c r="T11" s="53"/>
+      <c r="U11" s="53"/>
+      <c r="V11" s="53"/>
+      <c r="W11" s="53"/>
+      <c r="X11" s="53"/>
+      <c r="Y11" s="53"/>
+      <c r="Z11" s="53"/>
+      <c r="AA11" s="53"/>
+      <c r="AB11" s="53"/>
+      <c r="AC11" s="53"/>
+      <c r="AD11" s="53"/>
+      <c r="AE11" s="53"/>
+      <c r="AF11" s="53"/>
+      <c r="AG11" s="53"/>
+      <c r="AH11" s="54"/>
       <c r="AI11" s="12"/>
-      <c r="AJ11" s="54" t="s">
+      <c r="AJ11" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="AK11" s="54"/>
+      <c r="AK11" s="55"/>
       <c r="AL11" s="28"/>
       <c r="AM11" s="1"/>
       <c r="AN11" s="1"/>
@@ -4123,11 +4126,11 @@
       <c r="IV11" s="1"/>
     </row>
     <row r="12" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
       <c r="D12" s="18"/>
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
@@ -4160,10 +4163,10 @@
       <c r="AG12" s="19"/>
       <c r="AH12" s="19"/>
       <c r="AI12" s="11"/>
-      <c r="AJ12" s="39" t="s">
+      <c r="AJ12" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="AK12" s="40"/>
+      <c r="AK12" s="41"/>
       <c r="AL12" s="29"/>
       <c r="AM12" s="1"/>
       <c r="AN12" s="1"/>
@@ -4385,13 +4388,13 @@
       <c r="IV12" s="1"/>
     </row>
     <row r="13" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="43"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
@@ -4424,10 +4427,10 @@
       <c r="AG13" s="20"/>
       <c r="AH13" s="20"/>
       <c r="AI13" s="10"/>
-      <c r="AJ13" s="44" t="s">
+      <c r="AJ13" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="AK13" s="44"/>
+      <c r="AK13" s="45"/>
       <c r="AL13" s="30"/>
       <c r="AM13" s="1"/>
       <c r="AN13" s="1"/>
@@ -4649,11 +4652,11 @@
       <c r="IV13" s="1"/>
     </row>
     <row r="14" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A14" s="42"/>
-      <c r="B14" s="36" t="s">
+      <c r="A14" s="43"/>
+      <c r="B14" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="36"/>
+      <c r="C14" s="37"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -4686,10 +4689,10 @@
       <c r="AG14" s="6"/>
       <c r="AH14" s="6"/>
       <c r="AI14" s="6"/>
-      <c r="AJ14" s="36" t="s">
+      <c r="AJ14" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="AK14" s="36"/>
+      <c r="AK14" s="37"/>
       <c r="AL14" s="26"/>
       <c r="AM14" s="1"/>
       <c r="AN14" s="1"/>
@@ -4911,11 +4914,11 @@
       <c r="IV14" s="1"/>
     </row>
     <row r="15" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A15" s="42"/>
-      <c r="B15" s="36" t="s">
+      <c r="A15" s="43"/>
+      <c r="B15" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="36"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -4948,10 +4951,10 @@
       <c r="AG15" s="6"/>
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
-      <c r="AJ15" s="36" t="s">
+      <c r="AJ15" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="AK15" s="36"/>
+      <c r="AK15" s="37"/>
       <c r="AL15" s="26"/>
       <c r="AM15" s="1"/>
       <c r="AN15" s="1"/>
@@ -5173,11 +5176,11 @@
       <c r="IV15" s="1"/>
     </row>
     <row r="16" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A16" s="42"/>
-      <c r="B16" s="36" t="s">
+      <c r="A16" s="43"/>
+      <c r="B16" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="36"/>
+      <c r="C16" s="37"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -5210,10 +5213,10 @@
       <c r="AG16" s="6"/>
       <c r="AH16" s="6"/>
       <c r="AI16" s="6"/>
-      <c r="AJ16" s="36" t="s">
+      <c r="AJ16" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="AK16" s="36"/>
+      <c r="AK16" s="37"/>
       <c r="AL16" s="26"/>
       <c r="AM16" s="1"/>
       <c r="AN16" s="1"/>
@@ -5435,11 +5438,11 @@
       <c r="IV16" s="1"/>
     </row>
     <row r="17" spans="1:256" ht="24.9" customHeight="1">
-      <c r="A17" s="42"/>
-      <c r="B17" s="36" t="s">
+      <c r="A17" s="43"/>
+      <c r="B17" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="36"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -5472,10 +5475,10 @@
       <c r="AG17" s="6"/>
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
-      <c r="AJ17" s="36" t="s">
+      <c r="AJ17" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="AK17" s="36"/>
+      <c r="AK17" s="37"/>
       <c r="AL17" s="26"/>
       <c r="AM17" s="1"/>
       <c r="AN17" s="1"/>
@@ -5697,11 +5700,11 @@
       <c r="IV17" s="1"/>
     </row>
     <row r="18" spans="1:256" ht="24.75" customHeight="1">
-      <c r="A18" s="42"/>
-      <c r="B18" s="31" t="s">
+      <c r="A18" s="43"/>
+      <c r="B18" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="31"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -5734,10 +5737,10 @@
       <c r="AG18" s="6"/>
       <c r="AH18" s="6"/>
       <c r="AI18" s="6"/>
-      <c r="AJ18" s="31" t="s">
+      <c r="AJ18" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="AK18" s="31"/>
+      <c r="AK18" s="32"/>
       <c r="AL18" s="26"/>
       <c r="AM18" s="1"/>
       <c r="AN18" s="1"/>
@@ -5959,11 +5962,11 @@
       <c r="IV18" s="1"/>
     </row>
     <row r="19" spans="1:256" ht="24.75" customHeight="1">
-      <c r="A19" s="42"/>
-      <c r="B19" s="31" t="s">
+      <c r="A19" s="43"/>
+      <c r="B19" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="31"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -5996,10 +5999,10 @@
       <c r="AG19" s="6"/>
       <c r="AH19" s="6"/>
       <c r="AI19" s="6"/>
-      <c r="AJ19" s="31" t="s">
+      <c r="AJ19" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="AK19" s="31"/>
+      <c r="AK19" s="32"/>
       <c r="AL19" s="26"/>
       <c r="AM19" s="1"/>
       <c r="AN19" s="1"/>
@@ -6221,11 +6224,11 @@
       <c r="IV19" s="1"/>
     </row>
     <row r="20" spans="1:256" ht="24.75" customHeight="1">
-      <c r="A20" s="42"/>
-      <c r="B20" s="35" t="s">
+      <c r="A20" s="43"/>
+      <c r="B20" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="35"/>
+      <c r="C20" s="36"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -6258,8 +6261,8 @@
       <c r="AG20" s="6"/>
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
-      <c r="AJ20" s="32"/>
-      <c r="AK20" s="32"/>
+      <c r="AJ20" s="33"/>
+      <c r="AK20" s="33"/>
       <c r="AL20" s="26"/>
       <c r="AM20" s="1"/>
       <c r="AN20" s="1"/>
@@ -6481,45 +6484,45 @@
       <c r="IV20" s="1"/>
     </row>
     <row r="21" spans="1:256" ht="17.25" customHeight="1">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="37"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="37"/>
-      <c r="Q21" s="37"/>
-      <c r="R21" s="37"/>
-      <c r="S21" s="37"/>
-      <c r="T21" s="37"/>
-      <c r="U21" s="37"/>
-      <c r="V21" s="37"/>
-      <c r="W21" s="37"/>
-      <c r="X21" s="37"/>
-      <c r="Y21" s="37"/>
-      <c r="Z21" s="37"/>
-      <c r="AA21" s="37"/>
-      <c r="AB21" s="37"/>
-      <c r="AC21" s="37"/>
-      <c r="AD21" s="37"/>
-      <c r="AE21" s="37"/>
-      <c r="AF21" s="37"/>
-      <c r="AG21" s="37"/>
-      <c r="AH21" s="37"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="38"/>
+      <c r="R21" s="38"/>
+      <c r="S21" s="38"/>
+      <c r="T21" s="38"/>
+      <c r="U21" s="38"/>
+      <c r="V21" s="38"/>
+      <c r="W21" s="38"/>
+      <c r="X21" s="38"/>
+      <c r="Y21" s="38"/>
+      <c r="Z21" s="38"/>
+      <c r="AA21" s="38"/>
+      <c r="AB21" s="38"/>
+      <c r="AC21" s="38"/>
+      <c r="AD21" s="38"/>
+      <c r="AE21" s="38"/>
+      <c r="AF21" s="38"/>
+      <c r="AG21" s="38"/>
+      <c r="AH21" s="38"/>
       <c r="AI21" s="9"/>
-      <c r="AJ21" s="32"/>
-      <c r="AK21" s="32"/>
+      <c r="AJ21" s="33"/>
+      <c r="AK21" s="33"/>
       <c r="AL21" s="26"/>
       <c r="AM21" s="1"/>
       <c r="AN21" s="1"/>
@@ -6741,43 +6744,43 @@
       <c r="IV21" s="1"/>
     </row>
     <row r="22" spans="1:256" ht="15.75" customHeight="1">
-      <c r="A22" s="36"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="37"/>
-      <c r="Q22" s="37"/>
-      <c r="R22" s="37"/>
-      <c r="S22" s="37"/>
-      <c r="T22" s="37"/>
-      <c r="U22" s="37"/>
-      <c r="V22" s="37"/>
-      <c r="W22" s="37"/>
-      <c r="X22" s="37"/>
-      <c r="Y22" s="37"/>
-      <c r="Z22" s="37"/>
-      <c r="AA22" s="37"/>
-      <c r="AB22" s="37"/>
-      <c r="AC22" s="37"/>
-      <c r="AD22" s="37"/>
-      <c r="AE22" s="37"/>
-      <c r="AF22" s="37"/>
-      <c r="AG22" s="37"/>
-      <c r="AH22" s="37"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="38"/>
+      <c r="P22" s="38"/>
+      <c r="Q22" s="38"/>
+      <c r="R22" s="38"/>
+      <c r="S22" s="38"/>
+      <c r="T22" s="38"/>
+      <c r="U22" s="38"/>
+      <c r="V22" s="38"/>
+      <c r="W22" s="38"/>
+      <c r="X22" s="38"/>
+      <c r="Y22" s="38"/>
+      <c r="Z22" s="38"/>
+      <c r="AA22" s="38"/>
+      <c r="AB22" s="38"/>
+      <c r="AC22" s="38"/>
+      <c r="AD22" s="38"/>
+      <c r="AE22" s="38"/>
+      <c r="AF22" s="38"/>
+      <c r="AG22" s="38"/>
+      <c r="AH22" s="38"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="32"/>
-      <c r="AK22" s="32"/>
+      <c r="AJ22" s="33"/>
+      <c r="AK22" s="33"/>
       <c r="AL22" s="26"/>
       <c r="AM22" s="1"/>
       <c r="AN22" s="1"/>
@@ -6999,11 +7002,11 @@
       <c r="IV22" s="1"/>
     </row>
     <row r="23" spans="1:256" ht="18.75" customHeight="1">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -7036,8 +7039,8 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="32"/>
-      <c r="AK23" s="32"/>
+      <c r="AJ23" s="33"/>
+      <c r="AK23" s="33"/>
       <c r="AL23" s="26"/>
       <c r="AM23" s="1"/>
       <c r="AN23" s="1"/>
@@ -7259,47 +7262,47 @@
       <c r="IV23" s="1"/>
     </row>
     <row r="24" spans="1:256" ht="23.4" customHeight="1">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="33"/>
-      <c r="R24" s="33"/>
-      <c r="S24" s="33"/>
-      <c r="T24" s="33"/>
-      <c r="U24" s="33"/>
-      <c r="V24" s="33"/>
-      <c r="W24" s="33"/>
-      <c r="X24" s="33"/>
-      <c r="Y24" s="33"/>
-      <c r="Z24" s="33"/>
-      <c r="AA24" s="33"/>
-      <c r="AB24" s="33"/>
-      <c r="AC24" s="33"/>
-      <c r="AD24" s="33"/>
-      <c r="AE24" s="33"/>
-      <c r="AF24" s="33"/>
-      <c r="AG24" s="33"/>
-      <c r="AH24" s="33"/>
-      <c r="AI24" s="33"/>
-      <c r="AJ24" s="34" t="s">
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="34"/>
+      <c r="P24" s="34"/>
+      <c r="Q24" s="34"/>
+      <c r="R24" s="34"/>
+      <c r="S24" s="34"/>
+      <c r="T24" s="34"/>
+      <c r="U24" s="34"/>
+      <c r="V24" s="34"/>
+      <c r="W24" s="34"/>
+      <c r="X24" s="34"/>
+      <c r="Y24" s="34"/>
+      <c r="Z24" s="34"/>
+      <c r="AA24" s="34"/>
+      <c r="AB24" s="34"/>
+      <c r="AC24" s="34"/>
+      <c r="AD24" s="34"/>
+      <c r="AE24" s="34"/>
+      <c r="AF24" s="34"/>
+      <c r="AG24" s="34"/>
+      <c r="AH24" s="34"/>
+      <c r="AI24" s="34"/>
+      <c r="AJ24" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="AK24" s="34"/>
+      <c r="AK24" s="35"/>
       <c r="AL24" s="26"/>
       <c r="AM24" s="1"/>
       <c r="AN24" s="1"/>

</xml_diff>

<commit_message>
Work with HumanResources module
</commit_message>
<xml_diff>
--- a/GPERP_APP/Resources/Templates/Karta_pracy.xlsx
+++ b/GPERP_APP/Resources/Templates/Karta_pracy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\projekty GitHub\GlassPlant-ERP\GPERP_APP\Resources\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFA3C77-7781-449E-933F-31AF76BC1B29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5CF1B1-51C6-428A-A56D-DB32D560EEB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="936" windowWidth="18696" windowHeight="11424" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Karta" sheetId="4" r:id="rId1"/>

</xml_diff>